<commit_message>
Tuned level 6. Bug fix.
Fixed the bug where more than one level blocker would spawn at the same position.
</commit_message>
<xml_diff>
--- a/Tuning Matrix.xlsx
+++ b/Tuning Matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dorotea\UNITY PROJEKTI\Garden-Squad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89BB54A1-AC97-41DD-9BA7-99911A38435D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662C24B4-52F2-4C3F-B794-75491D150522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="21600" windowHeight="11385" xr2:uid="{BE3E6D60-BB80-41C6-9D40-86F64A4F08DB}"/>
+    <workbookView xWindow="1740" yWindow="1230" windowWidth="21600" windowHeight="11385" xr2:uid="{BE3E6D60-BB80-41C6-9D40-86F64A4F08DB}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="70">
   <si>
     <t>GARDEN DEFENSE - TUNING MATRIX</t>
   </si>
@@ -164,13 +164,94 @@
   </si>
   <si>
     <t>destroy scarecrow + deplete stars (to 0?)</t>
+  </si>
+  <si>
+    <t>LEVEL VALUES</t>
+  </si>
+  <si>
+    <t>stars</t>
+  </si>
+  <si>
+    <t>attack 1</t>
+  </si>
+  <si>
+    <t>attack 2</t>
+  </si>
+  <si>
+    <t>attack 3</t>
+  </si>
+  <si>
+    <t>attack 4</t>
+  </si>
+  <si>
+    <t>attack 5</t>
+  </si>
+  <si>
+    <t>stars mod</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Liz 3-4</t>
+  </si>
+  <si>
+    <t>Liz 2-4</t>
+  </si>
+  <si>
+    <t>Liz 3-5</t>
+  </si>
+  <si>
+    <t>Liz 3-7</t>
+  </si>
+  <si>
+    <t>Liz 4-10</t>
+  </si>
+  <si>
+    <t>Liz 5-5</t>
+  </si>
+  <si>
+    <t>Fox 5-7</t>
+  </si>
+  <si>
+    <t>Liz 7-10</t>
+  </si>
+  <si>
+    <t>Liz 5-8</t>
+  </si>
+  <si>
+    <t>Liz 8-10</t>
+  </si>
+  <si>
+    <t>Fox 5-8</t>
+  </si>
+  <si>
+    <t>Fox Liz 7-10</t>
+  </si>
+  <si>
+    <t>Fox 6-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blocked </t>
+  </si>
+  <si>
+    <t>Fox Liz 1-5</t>
+  </si>
+  <si>
+    <t>Liz Fox 5-10</t>
+  </si>
+  <si>
+    <t>Liz 1-8</t>
+  </si>
+  <si>
+    <t>Fox Liz 2-6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,8 +300,16 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,6 +319,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -261,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -272,6 +373,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -283,24 +413,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -635,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876C733A-4981-4C24-B368-D0A387520110}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,23 +759,24 @@
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="9" max="9" width="18.28515625" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -788,36 +901,36 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="12" t="s">
+      <c r="B7" s="9"/>
+      <c r="C7" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -867,12 +980,12 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -917,20 +1030,20 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="9"/>
-      <c r="F25" s="9" t="s">
+      <c r="B25" s="20"/>
+      <c r="F25" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="G25" s="9"/>
+      <c r="G25" s="20"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1000,7 +1113,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E33">
         <v>8</v>
       </c>
@@ -1008,12 +1121,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E34">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E35">
         <v>10</v>
       </c>
@@ -1021,8 +1134,225 @@
         <v>38</v>
       </c>
     </row>
+    <row r="37" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="14"/>
+      <c r="B38" s="15">
+        <v>1</v>
+      </c>
+      <c r="C38" s="15">
+        <v>2</v>
+      </c>
+      <c r="D38" s="15">
+        <v>3</v>
+      </c>
+      <c r="E38" s="15">
+        <v>4</v>
+      </c>
+      <c r="F38" s="15">
+        <v>5</v>
+      </c>
+      <c r="G38" s="15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="12">
+        <v>300</v>
+      </c>
+      <c r="C39" s="12">
+        <v>200</v>
+      </c>
+      <c r="D39" s="12">
+        <v>175</v>
+      </c>
+      <c r="E39" s="12">
+        <v>300</v>
+      </c>
+      <c r="F39" s="12">
+        <v>350</v>
+      </c>
+      <c r="G39" s="12">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" s="12">
+        <v>0</v>
+      </c>
+      <c r="C40" s="12">
+        <v>50</v>
+      </c>
+      <c r="D40" s="12">
+        <v>25</v>
+      </c>
+      <c r="E40" s="12">
+        <v>50</v>
+      </c>
+      <c r="F40" s="12">
+        <v>50</v>
+      </c>
+      <c r="G40" s="12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G46" s="12">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A37:G37"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="A15:D15"/>

</xml_diff>

<commit_message>
Added level 8. Initial setup level 8.
Introduced a new defender - scarecrow - repels foxes and lizards without taking or dealing damage.
Removed scarecrow button from UI in levels 1-4.
</commit_message>
<xml_diff>
--- a/Tuning Matrix.xlsx
+++ b/Tuning Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dorotea\UNITY PROJEKTI\Garden-Squad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662C24B4-52F2-4C3F-B794-75491D150522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F851C6A-8344-49C8-B66F-118180EAEA0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1740" yWindow="1230" windowWidth="21600" windowHeight="11385" xr2:uid="{BE3E6D60-BB80-41C6-9D40-86F64A4F08DB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="75">
   <si>
     <t>GARDEN DEFENSE - TUNING MATRIX</t>
   </si>
@@ -245,6 +245,21 @@
   </si>
   <si>
     <t>Fox Liz 2-6</t>
+  </si>
+  <si>
+    <t>Fox Liz 5-7</t>
+  </si>
+  <si>
+    <t>Ghastly 5-8</t>
+  </si>
+  <si>
+    <t>Liz Fox 7-10</t>
+  </si>
+  <si>
+    <t>Liz 3-6</t>
+  </si>
+  <si>
+    <t>Fox Liz 4-8</t>
   </si>
 </sst>
 </file>
@@ -750,7 +765,7 @@
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,6 +776,7 @@
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
     <col min="9" max="9" width="18.28515625" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
   </cols>
@@ -1113,7 +1129,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E33">
         <v>8</v>
       </c>
@@ -1121,12 +1137,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E34">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E35">
         <v>10</v>
       </c>
@@ -1134,7 +1150,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="16" t="s">
         <v>43</v>
       </c>
@@ -1145,7 +1161,7 @@
       <c r="F37" s="16"/>
       <c r="G37" s="16"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="14"/>
       <c r="B38" s="15">
         <v>1</v>
@@ -1165,8 +1181,11 @@
       <c r="G38" s="15">
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>44</v>
       </c>
@@ -1188,8 +1207,11 @@
       <c r="G39" s="12">
         <v>350</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>50</v>
       </c>
@@ -1211,8 +1233,11 @@
       <c r="G40" s="12">
         <v>50</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>45</v>
       </c>
@@ -1234,8 +1259,11 @@
       <c r="G41" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>46</v>
       </c>
@@ -1257,8 +1285,11 @@
       <c r="G42" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>47</v>
       </c>
@@ -1280,8 +1311,11 @@
       <c r="G43" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>48</v>
       </c>
@@ -1303,8 +1337,11 @@
       <c r="G44" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>49</v>
       </c>
@@ -1326,8 +1363,11 @@
       <c r="G45" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>65</v>
       </c>
@@ -1348,6 +1388,9 @@
       </c>
       <c r="G46" s="12">
         <v>3</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tuned level 8. Split attack from attacker movement.
Removed the scarecrow button from all levels up to level 8.
Cleaned up unused assets.
Removed attack logic from the attacker movement script into a separate script.
Set up the final attacker/boss - Golem.
</commit_message>
<xml_diff>
--- a/Tuning Matrix.xlsx
+++ b/Tuning Matrix.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dorotea\UNITY PROJEKTI\Garden-Squad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F851C6A-8344-49C8-B66F-118180EAEA0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA09C80E-8C8E-4407-8CBB-97CF51DC6A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="1230" windowWidth="21600" windowHeight="11385" xr2:uid="{BE3E6D60-BB80-41C6-9D40-86F64A4F08DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE3E6D60-BB80-41C6-9D40-86F64A4F08DB}"/>
   </bookViews>
   <sheets>
-    <sheet name="List1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tuning" sheetId="1" r:id="rId1"/>
+    <sheet name="Values" sheetId="2" r:id="rId2"/>
+    <sheet name="TODO" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="86">
   <si>
     <t>GARDEN DEFENSE - TUNING MATRIX</t>
   </si>
@@ -145,9 +147,6 @@
     <t>buy trophies - reduce starting stars: place trophy first</t>
   </si>
   <si>
-    <t>scarecrow + blockers (fox and lizard run away from scarecrow)</t>
-  </si>
-  <si>
     <t>introduce ghastly: can be killed, but passes through everything</t>
   </si>
   <si>
@@ -260,13 +259,49 @@
   </si>
   <si>
     <t>Fox Liz 4-8</t>
+  </si>
+  <si>
+    <t>audio</t>
+  </si>
+  <si>
+    <t>toggle countdown on/off</t>
+  </si>
+  <si>
+    <t>BACKLOG:</t>
+  </si>
+  <si>
+    <t>fade in/iris in level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">save/load level </t>
+  </si>
+  <si>
+    <t>level grid - locked/unlocked</t>
+  </si>
+  <si>
+    <t>TO DO:</t>
+  </si>
+  <si>
+    <t>game complete happy screen</t>
+  </si>
+  <si>
+    <t>credits screen</t>
+  </si>
+  <si>
+    <t>countdown before level starts (3 sec)</t>
+  </si>
+  <si>
+    <t>introduce scarecrow (fox and lizard run away from scarecrow)</t>
+  </si>
+  <si>
+    <t>buy scarecrow, blockers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,6 +354,22 @@
       <b/>
       <sz val="14"/>
       <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -377,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -414,9 +465,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -427,6 +475,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -762,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876C733A-4981-4C24-B368-D0A387520110}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,17 +839,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -823,7 +880,7 @@
         <v>11</v>
       </c>
       <c r="J3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -922,7 +979,7 @@
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -934,19 +991,19 @@
         <v>23</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -996,12 +1053,12 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -1046,20 +1103,20 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="20"/>
-      <c r="F25" s="20" t="s">
+      <c r="B25" s="19"/>
+      <c r="F25" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="G25" s="20"/>
+      <c r="G25" s="19"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1126,276 +1183,35 @@
         <v>7</v>
       </c>
       <c r="F32" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E33">
         <v>8</v>
       </c>
       <c r="F33" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E34">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E35">
         <v>10</v>
       </c>
       <c r="F35" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" s="16"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
-      <c r="B38" s="15">
-        <v>1</v>
-      </c>
-      <c r="C38" s="15">
-        <v>2</v>
-      </c>
-      <c r="D38" s="15">
-        <v>3</v>
-      </c>
-      <c r="E38" s="15">
-        <v>4</v>
-      </c>
-      <c r="F38" s="15">
-        <v>5</v>
-      </c>
-      <c r="G38" s="15">
-        <v>6</v>
-      </c>
-      <c r="H38" s="15">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" s="12">
-        <v>300</v>
-      </c>
-      <c r="C39" s="12">
-        <v>200</v>
-      </c>
-      <c r="D39" s="12">
-        <v>175</v>
-      </c>
-      <c r="E39" s="12">
-        <v>300</v>
-      </c>
-      <c r="F39" s="12">
-        <v>350</v>
-      </c>
-      <c r="G39" s="12">
-        <v>350</v>
-      </c>
-      <c r="H39" s="1">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B40" s="12">
-        <v>0</v>
-      </c>
-      <c r="C40" s="12">
-        <v>50</v>
-      </c>
-      <c r="D40" s="12">
-        <v>25</v>
-      </c>
-      <c r="E40" s="12">
-        <v>50</v>
-      </c>
-      <c r="F40" s="12">
-        <v>50</v>
-      </c>
-      <c r="G40" s="12">
-        <v>50</v>
-      </c>
-      <c r="H40" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G46" s="12">
-        <v>3</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A37:G37"/>
+  <mergeCells count="6">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="A15:D15"/>
@@ -1409,4 +1225,399 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{886BE5D4-24DB-4677-8687-FE4105B82910}">
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="15">
+        <v>1</v>
+      </c>
+      <c r="C2" s="15">
+        <v>2</v>
+      </c>
+      <c r="D2" s="15">
+        <v>3</v>
+      </c>
+      <c r="E2" s="15">
+        <v>4</v>
+      </c>
+      <c r="F2" s="15">
+        <v>5</v>
+      </c>
+      <c r="G2" s="15">
+        <v>6</v>
+      </c>
+      <c r="H2" s="15">
+        <v>7</v>
+      </c>
+      <c r="I2" s="15">
+        <v>8</v>
+      </c>
+      <c r="J2" s="15">
+        <v>9</v>
+      </c>
+      <c r="K2" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="12">
+        <v>300</v>
+      </c>
+      <c r="C3" s="12">
+        <v>200</v>
+      </c>
+      <c r="D3" s="12">
+        <v>175</v>
+      </c>
+      <c r="E3" s="12">
+        <v>300</v>
+      </c>
+      <c r="F3" s="12">
+        <v>350</v>
+      </c>
+      <c r="G3" s="12">
+        <v>350</v>
+      </c>
+      <c r="H3" s="1">
+        <v>350</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0</v>
+      </c>
+      <c r="C4" s="12">
+        <v>50</v>
+      </c>
+      <c r="D4" s="12">
+        <v>25</v>
+      </c>
+      <c r="E4" s="12">
+        <v>50</v>
+      </c>
+      <c r="F4" s="12">
+        <v>50</v>
+      </c>
+      <c r="G4" s="12">
+        <v>50</v>
+      </c>
+      <c r="H4" s="1">
+        <v>50</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="12">
+        <v>3</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00E65D11-134A-447B-8203-034CD728AF08}">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="G1" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="G1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Level 9 initial setup. Added countdown before start.
Level 9 - the player can buy the scarecrow defender.
Countdown (3 seconds) before the level starts. During this time, the game timer is paused, the attackers aren't spawning and the player can't buy any defenders.
</commit_message>
<xml_diff>
--- a/Tuning Matrix.xlsx
+++ b/Tuning Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dorotea\UNITY PROJEKTI\Garden-Squad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA09C80E-8C8E-4407-8CBB-97CF51DC6A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA7AF14-06EF-43A7-A7AB-7CFF47F3B318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE3E6D60-BB80-41C6-9D40-86F64A4F08DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{BE3E6D60-BB80-41C6-9D40-86F64A4F08DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tuning" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="90">
   <si>
     <t>GARDEN DEFENSE - TUNING MATRIX</t>
   </si>
@@ -264,9 +264,6 @@
     <t>audio</t>
   </si>
   <si>
-    <t>toggle countdown on/off</t>
-  </si>
-  <si>
     <t>BACKLOG:</t>
   </si>
   <si>
@@ -295,6 +292,21 @@
   </si>
   <si>
     <t>buy scarecrow, blockers</t>
+  </si>
+  <si>
+    <t>Liz Fox 8-9</t>
+  </si>
+  <si>
+    <t>Gh Fox 7-10</t>
+  </si>
+  <si>
+    <t>Liz 3-8</t>
+  </si>
+  <si>
+    <t>Scarecrow on 2</t>
+  </si>
+  <si>
+    <t>toggle countdown on/off, alt. Disabled automatically on difficulty lvl 3</t>
   </si>
 </sst>
 </file>
@@ -428,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -464,6 +476,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -821,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876C733A-4981-4C24-B368-D0A387520110}">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,17 +859,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -938,10 +958,10 @@
         <v>300</v>
       </c>
       <c r="H5">
-        <v>60</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
+        <v>250</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -998,12 +1018,12 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -1053,12 +1073,12 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -1074,7 +1094,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -1088,7 +1108,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -1102,23 +1122,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
+    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="J21" s="17"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="F25" s="19" t="s">
+      <c r="B25" s="23"/>
+      <c r="F25" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="G25" s="19"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="23"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1129,7 +1150,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1140,7 +1161,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1151,7 +1172,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1162,7 +1183,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E30">
         <v>5</v>
       </c>
@@ -1170,7 +1191,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E31">
         <v>6</v>
       </c>
@@ -1178,7 +1199,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E32">
         <v>7</v>
       </c>
@@ -1191,7 +1212,7 @@
         <v>8</v>
       </c>
       <c r="F33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="5:6" x14ac:dyDescent="0.25">
@@ -1199,7 +1220,7 @@
         <v>9</v>
       </c>
       <c r="F34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="5:6" x14ac:dyDescent="0.25">
@@ -1229,10 +1250,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{886BE5D4-24DB-4677-8687-FE4105B82910}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="K5" sqref="K5:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1245,15 +1266,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
@@ -1313,9 +1334,11 @@
       <c r="H3" s="1">
         <v>350</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="I3" s="1">
+        <v>300</v>
+      </c>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -1342,9 +1365,11 @@
       <c r="H4" s="1">
         <v>50</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="I4" s="1">
+        <v>30</v>
+      </c>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
@@ -1371,9 +1396,11 @@
       <c r="H5" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
@@ -1400,9 +1427,11 @@
       <c r="H6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
@@ -1429,9 +1458,11 @@
       <c r="H7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -1458,9 +1489,11 @@
       <c r="H8" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
@@ -1487,9 +1520,11 @@
       <c r="H9" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
+      <c r="I9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
@@ -1516,9 +1551,18 @@
       <c r="H10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
+      <c r="I10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J10" s="12">
+        <v>2</v>
+      </c>
+      <c r="K10" s="12"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I11" s="18" t="s">
+        <v>88</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1532,8 +1576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00E65D11-134A-447B-8203-034CD728AF08}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1542,17 +1586,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="G1" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="A1" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="G1" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -1565,7 +1609,7 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1573,13 +1617,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1587,13 +1631,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1601,7 +1645,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1609,7 +1653,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented fading between levels.
Set up animation with animation events on level controller object for fading between levels.
</commit_message>
<xml_diff>
--- a/Tuning Matrix.xlsx
+++ b/Tuning Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dorotea\UNITY PROJEKTI\Garden-Squad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA7AF14-06EF-43A7-A7AB-7CFF47F3B318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9680E39-803D-483C-A7B2-4B5314FE5A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{BE3E6D60-BB80-41C6-9D40-86F64A4F08DB}"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{BE3E6D60-BB80-41C6-9D40-86F64A4F08DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tuning" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="91">
   <si>
     <t>GARDEN DEFENSE - TUNING MATRIX</t>
   </si>
@@ -267,9 +267,6 @@
     <t>BACKLOG:</t>
   </si>
   <si>
-    <t>fade in/iris in level</t>
-  </si>
-  <si>
     <t xml:space="preserve">save/load level </t>
   </si>
   <si>
@@ -285,9 +282,6 @@
     <t>credits screen</t>
   </si>
   <si>
-    <t>countdown before level starts (3 sec)</t>
-  </si>
-  <si>
     <t>introduce scarecrow (fox and lizard run away from scarecrow)</t>
   </si>
   <si>
@@ -306,14 +300,49 @@
     <t>Scarecrow on 2</t>
   </si>
   <si>
-    <t>toggle countdown on/off, alt. Disabled automatically on difficulty lvl 3</t>
+    <t>toggle countdown on/off, alt. Disabled automatically on difficulty lvl 3?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">countdown before level starts (3 sec) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DONE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">fade in/iris in level </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DONE</t>
+    </r>
+  </si>
+  <si>
+    <t>level loading - currently not set up between levels</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,6 +411,14 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1212,7 +1249,7 @@
         <v>8</v>
       </c>
       <c r="F33" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="5:6" x14ac:dyDescent="0.25">
@@ -1220,7 +1257,7 @@
         <v>9</v>
       </c>
       <c r="F34" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="5:6" x14ac:dyDescent="0.25">
@@ -1428,7 +1465,7 @@
         <v>70</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
@@ -1459,7 +1496,7 @@
         <v>71</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
@@ -1490,7 +1527,7 @@
         <v>72</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
@@ -1561,7 +1598,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I11" s="18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1574,10 +1611,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00E65D11-134A-447B-8203-034CD728AF08}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1587,7 +1624,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -1609,7 +1646,7 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1617,13 +1654,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1631,13 +1668,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1645,7 +1682,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1653,7 +1690,15 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tuned lvl 9. Added countdown to all lvls.
</commit_message>
<xml_diff>
--- a/Tuning Matrix.xlsx
+++ b/Tuning Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dorotea\UNITY PROJEKTI\Garden-Squad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9680E39-803D-483C-A7B2-4B5314FE5A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62A8DEC-5875-4E8E-8F65-B014C789EBF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{BE3E6D60-BB80-41C6-9D40-86F64A4F08DB}"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="21600" windowHeight="11385" xr2:uid="{BE3E6D60-BB80-41C6-9D40-86F64A4F08DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tuning" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="96">
   <si>
     <t>GARDEN DEFENSE - TUNING MATRIX</t>
   </si>
@@ -283,9 +283,6 @@
   </si>
   <si>
     <t>introduce scarecrow (fox and lizard run away from scarecrow)</t>
-  </si>
-  <si>
-    <t>buy scarecrow, blockers</t>
   </si>
   <si>
     <t>Liz Fox 8-9</t>
@@ -336,6 +333,24 @@
   </si>
   <si>
     <t>level loading - currently not set up between levels</t>
+  </si>
+  <si>
+    <t>GFL 8-10</t>
+  </si>
+  <si>
+    <t>Liz Fox 7-9</t>
+  </si>
+  <si>
+    <t>Liz Fox 2-4</t>
+  </si>
+  <si>
+    <t>Liz Ghast 8-10</t>
+  </si>
+  <si>
+    <t>Ghastly 6-6</t>
+  </si>
+  <si>
+    <t>buy scarecrow, blockers: place scarecrow on 3 and trophies behind it</t>
   </si>
 </sst>
 </file>
@@ -450,7 +465,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -473,11 +488,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -543,6 +569,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalno" xfId="0" builtinId="0"/>
@@ -878,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876C733A-4981-4C24-B368-D0A387520110}">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1257,7 +1284,7 @@
         <v>9</v>
       </c>
       <c r="F34" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="5:6" x14ac:dyDescent="0.25">
@@ -1290,7 +1317,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:K10"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,7 +1401,9 @@
       <c r="I3" s="1">
         <v>300</v>
       </c>
-      <c r="J3" s="19"/>
+      <c r="J3" s="19">
+        <v>500</v>
+      </c>
       <c r="K3" s="19"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1405,7 +1434,9 @@
       <c r="I4" s="1">
         <v>30</v>
       </c>
-      <c r="J4" s="19"/>
+      <c r="J4" s="19">
+        <v>50</v>
+      </c>
       <c r="K4" s="19"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1436,7 +1467,9 @@
       <c r="I5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="J5" s="12"/>
+      <c r="J5" s="12" t="s">
+        <v>90</v>
+      </c>
       <c r="K5" s="12"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1465,9 +1498,11 @@
         <v>70</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="J6" s="12"/>
+        <v>82</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>93</v>
+      </c>
       <c r="K6" s="12"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1496,9 +1531,11 @@
         <v>71</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="J7" s="12"/>
+        <v>83</v>
+      </c>
+      <c r="J7" s="27" t="s">
+        <v>92</v>
+      </c>
       <c r="K7" s="12"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1527,9 +1564,11 @@
         <v>72</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="J8" s="12"/>
+        <v>84</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="K8" s="12"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1560,7 +1599,9 @@
       <c r="I9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J9" s="12"/>
+      <c r="J9" s="12" t="s">
+        <v>94</v>
+      </c>
       <c r="K9" s="12"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1598,7 +1639,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I11" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1613,8 +1654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00E65D11-134A-447B-8203-034CD728AF08}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1660,7 +1701,7 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1668,13 +1709,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1698,7 +1739,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Level 10 initial setup. Tuned boss stats.
</commit_message>
<xml_diff>
--- a/Tuning Matrix.xlsx
+++ b/Tuning Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dorotea\UNITY PROJEKTI\Garden-Squad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62A8DEC-5875-4E8E-8F65-B014C789EBF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850B4A67-B1A4-443E-8AA8-7A2569B1D120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="45" windowWidth="21600" windowHeight="11385" xr2:uid="{BE3E6D60-BB80-41C6-9D40-86F64A4F08DB}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="99">
   <si>
     <t>GARDEN DEFENSE - TUNING MATRIX</t>
   </si>
@@ -292,9 +292,6 @@
   </si>
   <si>
     <t>Liz 3-8</t>
-  </si>
-  <si>
-    <t>Scarecrow on 2</t>
   </si>
   <si>
     <t>toggle countdown on/off, alt. Disabled automatically on difficulty lvl 3?</t>
@@ -351,6 +348,18 @@
   </si>
   <si>
     <t>buy scarecrow, blockers: place scarecrow on 3 and trophies behind it</t>
+  </si>
+  <si>
+    <t>Scarecrow</t>
+  </si>
+  <si>
+    <t>on 2</t>
+  </si>
+  <si>
+    <t>buyable</t>
+  </si>
+  <si>
+    <t>2 set up, buyable</t>
   </si>
 </sst>
 </file>
@@ -503,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -570,6 +579,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalno" xfId="0" builtinId="0"/>
@@ -905,7 +918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876C733A-4981-4C24-B368-D0A387520110}">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
@@ -1284,7 +1297,7 @@
         <v>9</v>
       </c>
       <c r="F34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="5:6" x14ac:dyDescent="0.25">
@@ -1317,7 +1330,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1468,7 +1481,7 @@
         <v>70</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K5" s="12"/>
     </row>
@@ -1501,7 +1514,7 @@
         <v>82</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K6" s="12"/>
     </row>
@@ -1534,7 +1547,7 @@
         <v>83</v>
       </c>
       <c r="J7" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K7" s="12"/>
     </row>
@@ -1567,7 +1580,7 @@
         <v>84</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K8" s="12"/>
     </row>
@@ -1600,7 +1613,7 @@
         <v>68</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K9" s="12"/>
     </row>
@@ -1638,8 +1651,17 @@
       <c r="K10" s="12"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>95</v>
+      </c>
       <c r="I11" s="18" t="s">
-        <v>85</v>
+        <v>96</v>
+      </c>
+      <c r="J11" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="K11" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1701,7 +1723,7 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1709,13 +1731,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1739,7 +1761,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added StartNewGame button. Added the win screen,
</commit_message>
<xml_diff>
--- a/Tuning Matrix.xlsx
+++ b/Tuning Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dorotea\UNITY PROJEKTI\Garden-Squad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850B4A67-B1A4-443E-8AA8-7A2569B1D120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E522E495-CF0E-4C19-B7CF-8EC37A805FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="21600" windowHeight="11385" xr2:uid="{BE3E6D60-BB80-41C6-9D40-86F64A4F08DB}"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{BE3E6D60-BB80-41C6-9D40-86F64A4F08DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tuning" sheetId="1" r:id="rId1"/>
@@ -267,12 +267,6 @@
     <t>BACKLOG:</t>
   </si>
   <si>
-    <t xml:space="preserve">save/load level </t>
-  </si>
-  <si>
-    <t>level grid - locked/unlocked</t>
-  </si>
-  <si>
     <t>TO DO:</t>
   </si>
   <si>
@@ -329,9 +323,6 @@
     </r>
   </si>
   <si>
-    <t>level loading - currently not set up between levels</t>
-  </si>
-  <si>
     <t>GFL 8-10</t>
   </si>
   <si>
@@ -360,6 +351,54 @@
   </si>
   <si>
     <t>2 set up, buyable</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">level grid - locked/unlocked </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DONE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">level loading - currently not set up between levels </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DONE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">save/load level </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DONE</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -557,31 +596,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -918,7 +957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876C733A-4981-4C24-B368-D0A387520110}">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
@@ -936,17 +975,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1095,12 +1134,12 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -1150,12 +1189,12 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -1200,21 +1239,21 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
       <c r="J21" s="17"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="23"/>
-      <c r="F25" s="23" t="s">
+      <c r="B25" s="26"/>
+      <c r="F25" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="G25" s="23"/>
+      <c r="G25" s="26"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1289,7 +1328,7 @@
         <v>8</v>
       </c>
       <c r="F33" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="5:6" x14ac:dyDescent="0.25">
@@ -1297,7 +1336,7 @@
         <v>9</v>
       </c>
       <c r="F34" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="5:6" x14ac:dyDescent="0.25">
@@ -1343,15 +1382,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
@@ -1481,7 +1520,7 @@
         <v>70</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="K5" s="12"/>
     </row>
@@ -1511,10 +1550,10 @@
         <v>70</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K6" s="12"/>
     </row>
@@ -1544,10 +1583,10 @@
         <v>71</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="J7" s="27" t="s">
-        <v>91</v>
+        <v>81</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>88</v>
       </c>
       <c r="K7" s="12"/>
     </row>
@@ -1577,10 +1616,10 @@
         <v>72</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="K8" s="12"/>
     </row>
@@ -1613,7 +1652,7 @@
         <v>68</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="K9" s="12"/>
     </row>
@@ -1651,17 +1690,17 @@
       <c r="K10" s="12"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="J11" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="K11" t="s">
         <v>95</v>
-      </c>
-      <c r="I11" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="J11" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="K11" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1676,8 +1715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00E65D11-134A-447B-8203-034CD728AF08}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1686,17 +1725,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="G1" s="26" t="s">
+      <c r="A1" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="G1" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -1709,7 +1748,7 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1717,13 +1756,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1731,13 +1770,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1745,7 +1784,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1753,7 +1792,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1761,7 +1800,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>